<commit_message>
data provider and aftermethod relaunch the app if test fails
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shiva/Documents/FTAutomationFramework/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B751495C-9EF5-284B-845E-0DEDAE67F21F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B328AE4-416A-C443-8203-9B20F047BA98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15660" xr2:uid="{0C69E402-CEFD-CA4E-9B4A-AFD47945DA75}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15580" xr2:uid="{0C69E402-CEFD-CA4E-9B4A-AFD47945DA75}"/>
   </bookViews>
   <sheets>
     <sheet name="userIds" sheetId="1" r:id="rId1"/>
@@ -456,7 +456,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>